<commit_message>
Pooh Points: normal 20260217
</commit_message>
<xml_diff>
--- a/docs/Today_PoohPoints_SEC_ByOwner_2026-02-17.xlsx
+++ b/docs/Today_PoohPoints_SEC_ByOwner_2026-02-17.xlsx
@@ -597,14 +597,14 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>16:16 - 2nd Half</t>
+          <t>4:59 - 2nd Half</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="I2" t="n">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="J2" t="n">
         <v>9</v>
@@ -625,13 +625,13 @@
         <v>0</v>
       </c>
       <c r="P2" t="n">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="Q2" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="R2" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="S2" t="n">
         <v>0</v>
@@ -640,10 +640,10 @@
         <v>0</v>
       </c>
       <c r="U2" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="V2" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
@@ -664,68 +664,68 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Tramon Mark</t>
+          <t>Jeremiah Wilkinson</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>TEX</t>
+          <t>UGA</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>LSU@TEX</t>
+          <t>UGA@UK</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>16:16 - 2nd Half</t>
+          <t>10:55 - 2nd Half</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="I3" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="J3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M3" t="n">
         <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P3" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="Q3" t="n">
+        <v>5</v>
+      </c>
+      <c r="R3" t="n">
+        <v>13</v>
+      </c>
+      <c r="S3" t="n">
+        <v>3</v>
+      </c>
+      <c r="T3" t="n">
+        <v>7</v>
+      </c>
+      <c r="U3" t="n">
+        <v>3</v>
+      </c>
+      <c r="V3" t="n">
         <v>4</v>
-      </c>
-      <c r="R3" t="n">
-        <v>7</v>
-      </c>
-      <c r="S3" t="n">
-        <v>2</v>
-      </c>
-      <c r="T3" t="n">
-        <v>3</v>
-      </c>
-      <c r="U3" t="n">
-        <v>0</v>
-      </c>
-      <c r="V3" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -746,68 +746,68 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Jeremiah Wilkinson</t>
+          <t>Tramon Mark</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>UGA</t>
+          <t>TEX</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>UGA@UK</t>
+          <t>LSU@TEX</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Halftime</t>
+          <t>4:59 - 2nd Half</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="I4" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="J4" t="n">
         <v>2</v>
       </c>
       <c r="K4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M4" t="n">
         <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P4" t="n">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="Q4" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="R4" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="S4" t="n">
         <v>2</v>
       </c>
       <c r="T4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -843,14 +843,14 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>16:16 - 2nd Half</t>
+          <t>4:59 - 2nd Half</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J5" t="n">
         <v>3</v>
@@ -859,7 +859,7 @@
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5" t="n">
         <v>1</v>
@@ -871,13 +871,13 @@
         <v>3</v>
       </c>
       <c r="P5" t="n">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="Q5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S5" t="n">
         <v>0</v>
@@ -1171,11 +1171,11 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Halftime</t>
+          <t>10:55 - 2nd Half</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I9" t="n">
         <v>4</v>
@@ -1184,7 +1184,7 @@
         <v>1</v>
       </c>
       <c r="K9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L9" t="n">
         <v>0</v>
@@ -1196,22 +1196,22 @@
         <v>0</v>
       </c>
       <c r="O9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P9" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="Q9" t="n">
         <v>2</v>
       </c>
       <c r="R9" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S9" t="n">
         <v>0</v>
       </c>
       <c r="T9" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="U9" t="n">
         <v>0</v>
@@ -1253,47 +1253,47 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Halftime</t>
+          <t>10:55 - 2nd Half</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="I10" t="n">
+        <v>12</v>
+      </c>
+      <c r="J10" t="n">
+        <v>2</v>
+      </c>
+      <c r="K10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="n">
+        <v>1</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>4</v>
+      </c>
+      <c r="R10" t="n">
         <v>6</v>
       </c>
-      <c r="J10" t="n">
-        <v>1</v>
-      </c>
-      <c r="K10" t="n">
-        <v>1</v>
-      </c>
-      <c r="L10" t="n">
-        <v>0</v>
-      </c>
-      <c r="M10" t="n">
-        <v>0</v>
-      </c>
-      <c r="N10" t="n">
-        <v>1</v>
-      </c>
-      <c r="O10" t="n">
-        <v>0</v>
-      </c>
-      <c r="P10" t="n">
-        <v>14</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>2</v>
-      </c>
-      <c r="R10" t="n">
-        <v>2</v>
-      </c>
       <c r="S10" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T10" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="U10" t="n">
         <v>0</v>
@@ -1417,17 +1417,17 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>16:16 - 2nd Half</t>
+          <t>4:59 - 2nd Half</t>
         </is>
       </c>
       <c r="H12" t="n">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="I12" t="n">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="J12" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K12" t="n">
         <v>0</v>
@@ -1442,28 +1442,28 @@
         <v>1</v>
       </c>
       <c r="O12" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P12" t="n">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="Q12" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R12" t="n">
+        <v>9</v>
+      </c>
+      <c r="S12" t="n">
+        <v>1</v>
+      </c>
+      <c r="T12" t="n">
+        <v>2</v>
+      </c>
+      <c r="U12" t="n">
         <v>8</v>
       </c>
-      <c r="S12" t="n">
-        <v>0</v>
-      </c>
-      <c r="T12" t="n">
-        <v>1</v>
-      </c>
-      <c r="U12" t="n">
-        <v>6</v>
-      </c>
       <c r="V12" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13">
@@ -1499,20 +1499,20 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Halftime</t>
+          <t>10:55 - 2nd Half</t>
         </is>
       </c>
       <c r="H13" t="n">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="I13" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="J13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K13" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L13" t="n">
         <v>0</v>
@@ -1521,31 +1521,31 @@
         <v>0</v>
       </c>
       <c r="N13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O13" t="n">
         <v>0</v>
       </c>
       <c r="P13" t="n">
+        <v>25</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>10</v>
+      </c>
+      <c r="R13" t="n">
         <v>16</v>
       </c>
-      <c r="Q13" t="n">
+      <c r="S13" t="n">
+        <v>3</v>
+      </c>
+      <c r="T13" t="n">
         <v>5</v>
       </c>
-      <c r="R13" t="n">
-        <v>11</v>
-      </c>
-      <c r="S13" t="n">
-        <v>1</v>
-      </c>
-      <c r="T13" t="n">
-        <v>3</v>
-      </c>
       <c r="U13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V13" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14">
@@ -1745,17 +1745,17 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Halftime</t>
+          <t>10:55 - 2nd Half</t>
         </is>
       </c>
       <c r="H16" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I16" t="n">
         <v>4</v>
       </c>
       <c r="J16" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K16" t="n">
         <v>0</v>
@@ -1764,7 +1764,7 @@
         <v>0</v>
       </c>
       <c r="M16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N16" t="n">
         <v>3</v>
@@ -1773,7 +1773,7 @@
         <v>1</v>
       </c>
       <c r="P16" t="n">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="Q16" t="n">
         <v>1</v>
@@ -1812,68 +1812,68 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Jordan Pope</t>
+          <t>Somtochukwu Cyril</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>TEX</t>
+          <t>UGA</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>LSU@TEX</t>
+          <t>UGA@UK</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>16:16 - 2nd Half</t>
+          <t>10:55 - 2nd Half</t>
         </is>
       </c>
       <c r="H17" t="n">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="I17" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J17" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="K17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17" t="n">
         <v>1</v>
       </c>
       <c r="M17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O17" t="n">
         <v>1</v>
       </c>
       <c r="P17" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="Q17" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R17" t="n">
         <v>6</v>
       </c>
       <c r="S17" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="T17" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="U17" t="n">
         <v>2</v>
       </c>
       <c r="V17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18">
@@ -1894,68 +1894,68 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Somtochukwu Cyril</t>
+          <t>Jordan Pope</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>UGA</t>
+          <t>TEX</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>UGA@UK</t>
+          <t>LSU@TEX</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Halftime</t>
+          <t>4:59 - 2nd Half</t>
         </is>
       </c>
       <c r="H18" t="n">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="I18" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="J18" t="n">
+        <v>2</v>
+      </c>
+      <c r="K18" t="n">
+        <v>1</v>
+      </c>
+      <c r="L18" t="n">
+        <v>1</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0</v>
+      </c>
+      <c r="O18" t="n">
+        <v>1</v>
+      </c>
+      <c r="P18" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q18" t="n">
         <v>4</v>
       </c>
-      <c r="K18" t="n">
-        <v>0</v>
-      </c>
-      <c r="L18" t="n">
-        <v>1</v>
-      </c>
-      <c r="M18" t="n">
-        <v>1</v>
-      </c>
-      <c r="N18" t="n">
-        <v>1</v>
-      </c>
-      <c r="O18" t="n">
-        <v>0</v>
-      </c>
-      <c r="P18" t="n">
-        <v>12</v>
-      </c>
-      <c r="Q18" t="n">
-        <v>3</v>
-      </c>
       <c r="R18" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="S18" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T18" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U18" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="V18" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19">
@@ -1976,62 +1976,62 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Xaivian Lee</t>
+          <t>Mike Nwoko</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>FLA</t>
+          <t>LSU</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>SC@FLA</t>
+          <t>LSU@TEX</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Final</t>
+          <t>4:59 - 2nd Half</t>
         </is>
       </c>
       <c r="H19" t="n">
         <v>8</v>
       </c>
       <c r="I19" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="J19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K19" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N19" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="O19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P19" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="Q19" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="R19" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="S19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T19" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="U19" t="n">
         <v>0</v>
@@ -2058,62 +2058,62 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Mike Nwoko</t>
+          <t>Xaivian Lee</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>LSU</t>
+          <t>FLA</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>LSU@TEX</t>
+          <t>SC@FLA</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>16:16 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H20" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I20" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N20" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O20" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P20" t="n">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="Q20" t="n">
         <v>4</v>
       </c>
       <c r="R20" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="S20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T20" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U20" t="n">
         <v>0</v>
@@ -2222,38 +2222,38 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Dailyn Swain</t>
+          <t>Blue Cain</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>TEX</t>
+          <t>UGA</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>LSU@TEX</t>
+          <t>UGA@UK</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>16:16 - 2nd Half</t>
+          <t>10:55 - 2nd Half</t>
         </is>
       </c>
       <c r="H22" t="n">
         <v>21</v>
       </c>
       <c r="I22" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J22" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L22" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M22" t="n">
         <v>0</v>
@@ -2262,28 +2262,28 @@
         <v>1</v>
       </c>
       <c r="O22" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P22" t="n">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="Q22" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R22" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="S22" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T22" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="U22" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V22" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23">
@@ -2304,68 +2304,68 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Blue Cain</t>
+          <t>Dailyn Swain</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>UGA</t>
+          <t>TEX</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>UGA@UK</t>
+          <t>LSU@TEX</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Halftime</t>
+          <t>4:59 - 2nd Half</t>
         </is>
       </c>
       <c r="H23" t="n">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="I23" t="n">
+        <v>19</v>
+      </c>
+      <c r="J23" t="n">
         <v>9</v>
       </c>
-      <c r="J23" t="n">
-        <v>2</v>
-      </c>
       <c r="K23" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L23" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M23" t="n">
         <v>0</v>
       </c>
       <c r="N23" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O23" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P23" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="Q23" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="R23" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="S23" t="n">
         <v>1</v>
       </c>
       <c r="T23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U23" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="V23" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24">
@@ -2401,21 +2401,21 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Halftime</t>
+          <t>10:55 - 2nd Half</t>
         </is>
       </c>
       <c r="H24" t="n">
+        <v>16</v>
+      </c>
+      <c r="I24" t="n">
         <v>9</v>
       </c>
-      <c r="I24" t="n">
+      <c r="J24" t="n">
+        <v>1</v>
+      </c>
+      <c r="K24" t="n">
         <v>6</v>
       </c>
-      <c r="J24" t="n">
-        <v>1</v>
-      </c>
-      <c r="K24" t="n">
-        <v>2</v>
-      </c>
       <c r="L24" t="n">
         <v>1</v>
       </c>
@@ -2426,22 +2426,22 @@
         <v>0</v>
       </c>
       <c r="O24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P24" t="n">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="Q24" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R24" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S24" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T24" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U24" t="n">
         <v>0</v>
@@ -2468,32 +2468,32 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Kobe Knox</t>
+          <t>Mouhamed Dioubate</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>SC</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>SC@FLA</t>
+          <t>UGA@UK</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Final</t>
+          <t>10:55 - 2nd Half</t>
         </is>
       </c>
       <c r="H25" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I25" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="J25" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K25" t="n">
         <v>1</v>
@@ -2505,25 +2505,25 @@
         <v>0</v>
       </c>
       <c r="N25" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O25" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P25" t="n">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="Q25" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="R25" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="S25" t="n">
         <v>0</v>
       </c>
       <c r="T25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U25" t="n">
         <v>1</v>
@@ -2550,68 +2550,68 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Mouhamed Dioubate</t>
+          <t>Kobe Knox</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>UK</t>
+          <t>SC</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>UGA@UK</t>
+          <t>SC@FLA</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Halftime</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H26" t="n">
         <v>4</v>
       </c>
       <c r="I26" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J26" t="n">
+        <v>1</v>
+      </c>
+      <c r="K26" t="n">
+        <v>1</v>
+      </c>
+      <c r="L26" t="n">
+        <v>0</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0</v>
+      </c>
+      <c r="N26" t="n">
+        <v>2</v>
+      </c>
+      <c r="O26" t="n">
+        <v>1</v>
+      </c>
+      <c r="P26" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q26" t="n">
         <v>4</v>
       </c>
-      <c r="K26" t="n">
-        <v>0</v>
-      </c>
-      <c r="L26" t="n">
-        <v>0</v>
-      </c>
-      <c r="M26" t="n">
-        <v>0</v>
-      </c>
-      <c r="N26" t="n">
-        <v>0</v>
-      </c>
-      <c r="O26" t="n">
-        <v>2</v>
-      </c>
-      <c r="P26" t="n">
-        <v>7</v>
-      </c>
-      <c r="Q26" t="n">
-        <v>0</v>
-      </c>
       <c r="R26" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="S26" t="n">
         <v>0</v>
       </c>
       <c r="T26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V26" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27">
@@ -2647,20 +2647,20 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>16:16 - 2nd Half</t>
+          <t>4:59 - 2nd Half</t>
         </is>
       </c>
       <c r="H27" t="n">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="I27" t="n">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="J27" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K27" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L27" t="n">
         <v>0</v>
@@ -2669,31 +2669,31 @@
         <v>0</v>
       </c>
       <c r="N27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O27" t="n">
         <v>1</v>
       </c>
       <c r="P27" t="n">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="Q27" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="R27" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="S27" t="n">
         <v>1</v>
       </c>
       <c r="T27" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
@@ -2811,47 +2811,47 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>16:16 - 2nd Half</t>
+          <t>4:59 - 2nd Half</t>
         </is>
       </c>
       <c r="H29" t="n">
+        <v>16</v>
+      </c>
+      <c r="I29" t="n">
         <v>12</v>
       </c>
-      <c r="I29" t="n">
-        <v>9</v>
-      </c>
       <c r="J29" t="n">
         <v>2</v>
       </c>
       <c r="K29" t="n">
+        <v>7</v>
+      </c>
+      <c r="L29" t="n">
+        <v>2</v>
+      </c>
+      <c r="M29" t="n">
+        <v>0</v>
+      </c>
+      <c r="N29" t="n">
+        <v>1</v>
+      </c>
+      <c r="O29" t="n">
+        <v>3</v>
+      </c>
+      <c r="P29" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q29" t="n">
         <v>4</v>
       </c>
-      <c r="L29" t="n">
-        <v>2</v>
-      </c>
-      <c r="M29" t="n">
-        <v>0</v>
-      </c>
-      <c r="N29" t="n">
-        <v>1</v>
-      </c>
-      <c r="O29" t="n">
-        <v>2</v>
-      </c>
-      <c r="P29" t="n">
-        <v>23</v>
-      </c>
-      <c r="Q29" t="n">
-        <v>3</v>
-      </c>
       <c r="R29" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="S29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T29" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U29" t="n">
         <v>2</v>
@@ -2893,23 +2893,23 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>16:16 - 2nd Half</t>
+          <t>4:59 - 2nd Half</t>
         </is>
       </c>
       <c r="H30" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I30" t="n">
         <v>4</v>
       </c>
       <c r="J30" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K30" t="n">
         <v>1</v>
       </c>
       <c r="L30" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M30" t="n">
         <v>2</v>
@@ -2918,10 +2918,10 @@
         <v>0</v>
       </c>
       <c r="O30" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P30" t="n">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="Q30" t="n">
         <v>2</v>
@@ -2960,29 +2960,29 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Elijah Strong</t>
+          <t>Camden Heide</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>SC</t>
+          <t>TEX</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>SC@FLA</t>
+          <t>LSU@TEX</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Final</t>
+          <t>4:59 - 2nd Half</t>
         </is>
       </c>
       <c r="H31" t="n">
         <v>8</v>
       </c>
       <c r="I31" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J31" t="n">
         <v>3</v>
@@ -2997,31 +2997,31 @@
         <v>0</v>
       </c>
       <c r="N31" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O31" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P31" t="n">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="Q31" t="n">
+        <v>3</v>
+      </c>
+      <c r="R31" t="n">
         <v>5</v>
       </c>
-      <c r="R31" t="n">
-        <v>8</v>
-      </c>
       <c r="S31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T31" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V31" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32">
@@ -3042,41 +3042,41 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Christ Essandoko</t>
+          <t>Dylan James</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>SC</t>
+          <t>UGA</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>SC@FLA</t>
+          <t>UGA@UK</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Final</t>
+          <t>10:55 - 2nd Half</t>
         </is>
       </c>
       <c r="H32" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I32" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J32" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K32" t="n">
         <v>1</v>
       </c>
       <c r="L32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M32" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N32" t="n">
         <v>0</v>
@@ -3085,7 +3085,7 @@
         <v>0</v>
       </c>
       <c r="P32" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="Q32" t="n">
         <v>2</v>
@@ -3097,13 +3097,13 @@
         <v>0</v>
       </c>
       <c r="T32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U32" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V32" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -3124,62 +3124,62 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Dylan James</t>
+          <t>Elijah Strong</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>UGA</t>
+          <t>SC</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>UGA@UK</t>
+          <t>SC@FLA</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Halftime</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H33" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I33" t="n">
+        <v>10</v>
+      </c>
+      <c r="J33" t="n">
+        <v>3</v>
+      </c>
+      <c r="K33" t="n">
+        <v>0</v>
+      </c>
+      <c r="L33" t="n">
+        <v>0</v>
+      </c>
+      <c r="M33" t="n">
+        <v>0</v>
+      </c>
+      <c r="N33" t="n">
+        <v>2</v>
+      </c>
+      <c r="O33" t="n">
         <v>4</v>
       </c>
-      <c r="J33" t="n">
-        <v>1</v>
-      </c>
-      <c r="K33" t="n">
-        <v>0</v>
-      </c>
-      <c r="L33" t="n">
-        <v>0</v>
-      </c>
-      <c r="M33" t="n">
-        <v>2</v>
-      </c>
-      <c r="N33" t="n">
-        <v>0</v>
-      </c>
-      <c r="O33" t="n">
-        <v>0</v>
-      </c>
       <c r="P33" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="Q33" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="R33" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="S33" t="n">
         <v>0</v>
       </c>
       <c r="T33" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U33" t="n">
         <v>0</v>
@@ -3206,68 +3206,68 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Eli Ellis</t>
+          <t>Jake Wilkins</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>SC</t>
+          <t>UGA</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>SC@FLA</t>
+          <t>UGA@UK</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Final</t>
+          <t>10:55 - 2nd Half</t>
         </is>
       </c>
       <c r="H34" t="n">
+        <v>8</v>
+      </c>
+      <c r="I34" t="n">
         <v>6</v>
       </c>
-      <c r="I34" t="n">
+      <c r="J34" t="n">
+        <v>3</v>
+      </c>
+      <c r="K34" t="n">
+        <v>1</v>
+      </c>
+      <c r="L34" t="n">
+        <v>0</v>
+      </c>
+      <c r="M34" t="n">
+        <v>0</v>
+      </c>
+      <c r="N34" t="n">
+        <v>0</v>
+      </c>
+      <c r="O34" t="n">
+        <v>1</v>
+      </c>
+      <c r="P34" t="n">
+        <v>9</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>2</v>
+      </c>
+      <c r="R34" t="n">
         <v>4</v>
       </c>
-      <c r="J34" t="n">
-        <v>2</v>
-      </c>
-      <c r="K34" t="n">
-        <v>3</v>
-      </c>
-      <c r="L34" t="n">
-        <v>1</v>
-      </c>
-      <c r="M34" t="n">
-        <v>0</v>
-      </c>
-      <c r="N34" t="n">
-        <v>0</v>
-      </c>
-      <c r="O34" t="n">
-        <v>2</v>
-      </c>
-      <c r="P34" t="n">
-        <v>29</v>
-      </c>
-      <c r="Q34" t="n">
-        <v>2</v>
-      </c>
-      <c r="R34" t="n">
-        <v>6</v>
-      </c>
       <c r="S34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T34" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="U34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
@@ -3288,12 +3288,12 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Urban Klavzar</t>
+          <t>Christ Essandoko</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>FLA</t>
+          <t>SC</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3307,49 +3307,49 @@
         </is>
       </c>
       <c r="H35" t="n">
+        <v>7</v>
+      </c>
+      <c r="I35" t="n">
+        <v>6</v>
+      </c>
+      <c r="J35" t="n">
+        <v>3</v>
+      </c>
+      <c r="K35" t="n">
+        <v>1</v>
+      </c>
+      <c r="L35" t="n">
+        <v>1</v>
+      </c>
+      <c r="M35" t="n">
+        <v>0</v>
+      </c>
+      <c r="N35" t="n">
+        <v>0</v>
+      </c>
+      <c r="O35" t="n">
+        <v>0</v>
+      </c>
+      <c r="P35" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>2</v>
+      </c>
+      <c r="R35" t="n">
+        <v>3</v>
+      </c>
+      <c r="S35" t="n">
+        <v>0</v>
+      </c>
+      <c r="T35" t="n">
+        <v>1</v>
+      </c>
+      <c r="U35" t="n">
+        <v>2</v>
+      </c>
+      <c r="V35" t="n">
         <v>5</v>
-      </c>
-      <c r="I35" t="n">
-        <v>5</v>
-      </c>
-      <c r="J35" t="n">
-        <v>3</v>
-      </c>
-      <c r="K35" t="n">
-        <v>0</v>
-      </c>
-      <c r="L35" t="n">
-        <v>0</v>
-      </c>
-      <c r="M35" t="n">
-        <v>0</v>
-      </c>
-      <c r="N35" t="n">
-        <v>0</v>
-      </c>
-      <c r="O35" t="n">
-        <v>4</v>
-      </c>
-      <c r="P35" t="n">
-        <v>17</v>
-      </c>
-      <c r="Q35" t="n">
-        <v>2</v>
-      </c>
-      <c r="R35" t="n">
-        <v>5</v>
-      </c>
-      <c r="S35" t="n">
-        <v>1</v>
-      </c>
-      <c r="T35" t="n">
-        <v>4</v>
-      </c>
-      <c r="U35" t="n">
-        <v>0</v>
-      </c>
-      <c r="V35" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -3385,17 +3385,17 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Halftime</t>
+          <t>10:55 - 2nd Half</t>
         </is>
       </c>
       <c r="H36" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I36" t="n">
         <v>4</v>
       </c>
       <c r="J36" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K36" t="n">
         <v>0</v>
@@ -3410,10 +3410,10 @@
         <v>2</v>
       </c>
       <c r="O36" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P36" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Q36" t="n">
         <v>2</v>
@@ -3452,68 +3452,68 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Camden Heide</t>
+          <t>Eli Ellis</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>TEX</t>
+          <t>SC</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>LSU@TEX</t>
+          <t>SC@FLA</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>16:16 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H37" t="n">
+        <v>6</v>
+      </c>
+      <c r="I37" t="n">
         <v>4</v>
       </c>
-      <c r="I37" t="n">
+      <c r="J37" t="n">
+        <v>2</v>
+      </c>
+      <c r="K37" t="n">
+        <v>3</v>
+      </c>
+      <c r="L37" t="n">
+        <v>1</v>
+      </c>
+      <c r="M37" t="n">
+        <v>0</v>
+      </c>
+      <c r="N37" t="n">
+        <v>0</v>
+      </c>
+      <c r="O37" t="n">
+        <v>2</v>
+      </c>
+      <c r="P37" t="n">
+        <v>29</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>2</v>
+      </c>
+      <c r="R37" t="n">
         <v>6</v>
       </c>
-      <c r="J37" t="n">
-        <v>1</v>
-      </c>
-      <c r="K37" t="n">
-        <v>0</v>
-      </c>
-      <c r="L37" t="n">
-        <v>0</v>
-      </c>
-      <c r="M37" t="n">
-        <v>0</v>
-      </c>
-      <c r="N37" t="n">
-        <v>0</v>
-      </c>
-      <c r="O37" t="n">
-        <v>2</v>
-      </c>
-      <c r="P37" t="n">
-        <v>23</v>
-      </c>
-      <c r="Q37" t="n">
-        <v>2</v>
-      </c>
-      <c r="R37" t="n">
-        <v>4</v>
-      </c>
       <c r="S37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T37" t="n">
         <v>3</v>
       </c>
       <c r="U37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V37" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -3534,7 +3534,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Chendall Weaver</t>
+          <t>Simeon Wilcher</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -3549,53 +3549,53 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>16:16 - 2nd Half</t>
+          <t>4:59 - 2nd Half</t>
         </is>
       </c>
       <c r="H38" t="n">
+        <v>6</v>
+      </c>
+      <c r="I38" t="n">
         <v>4</v>
       </c>
-      <c r="I38" t="n">
-        <v>2</v>
-      </c>
       <c r="J38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K38" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L38" t="n">
         <v>0</v>
       </c>
       <c r="M38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O38" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P38" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="Q38" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R38" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S38" t="n">
         <v>0</v>
       </c>
       <c r="T38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U38" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V38" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -3616,62 +3616,62 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Simeon Wilcher</t>
+          <t>Urban Klavzar</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>TEX</t>
+          <t>FLA</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>LSU@TEX</t>
+          <t>SC@FLA</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>16:16 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H39" t="n">
+        <v>5</v>
+      </c>
+      <c r="I39" t="n">
+        <v>5</v>
+      </c>
+      <c r="J39" t="n">
+        <v>3</v>
+      </c>
+      <c r="K39" t="n">
+        <v>0</v>
+      </c>
+      <c r="L39" t="n">
+        <v>0</v>
+      </c>
+      <c r="M39" t="n">
+        <v>0</v>
+      </c>
+      <c r="N39" t="n">
+        <v>0</v>
+      </c>
+      <c r="O39" t="n">
         <v>4</v>
       </c>
-      <c r="I39" t="n">
-        <v>2</v>
-      </c>
-      <c r="J39" t="n">
-        <v>0</v>
-      </c>
-      <c r="K39" t="n">
-        <v>3</v>
-      </c>
-      <c r="L39" t="n">
-        <v>0</v>
-      </c>
-      <c r="M39" t="n">
-        <v>0</v>
-      </c>
-      <c r="N39" t="n">
-        <v>1</v>
-      </c>
-      <c r="O39" t="n">
-        <v>0</v>
-      </c>
       <c r="P39" t="n">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="Q39" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R39" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="S39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T39" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U39" t="n">
         <v>0</v>
@@ -3698,32 +3698,32 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Eli Sparkman</t>
+          <t>Chendall Weaver</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>SC</t>
+          <t>TEX</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>SC@FLA</t>
+          <t>LSU@TEX</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Final</t>
+          <t>4:59 - 2nd Half</t>
         </is>
       </c>
       <c r="H40" t="n">
         <v>3</v>
       </c>
       <c r="I40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K40" t="n">
         <v>0</v>
@@ -3732,7 +3732,7 @@
         <v>0</v>
       </c>
       <c r="M40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N40" t="n">
         <v>0</v>
@@ -3741,25 +3741,25 @@
         <v>0</v>
       </c>
       <c r="P40" t="n">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="Q40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R40" t="n">
         <v>1</v>
       </c>
       <c r="S40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U40" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V40" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41">
@@ -3780,22 +3780,22 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Jake Wilkins</t>
+          <t>Eli Sparkman</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>UGA</t>
+          <t>SC</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>UGA@UK</t>
+          <t>SC@FLA</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Halftime</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H41" t="n">
@@ -3805,10 +3805,10 @@
         <v>3</v>
       </c>
       <c r="J41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L41" t="n">
         <v>0</v>
@@ -3820,16 +3820,16 @@
         <v>0</v>
       </c>
       <c r="O41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P41" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="Q41" t="n">
         <v>1</v>
       </c>
       <c r="R41" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="S41" t="n">
         <v>1</v>
@@ -3862,29 +3862,29 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Hayden Assemian</t>
+          <t>Brandon Garrison</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>SC</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>SC@FLA</t>
+          <t>UGA@UK</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Final</t>
+          <t>10:55 - 2nd Half</t>
         </is>
       </c>
       <c r="H42" t="n">
         <v>2</v>
       </c>
       <c r="I42" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J42" t="n">
         <v>3</v>
@@ -3899,28 +3899,28 @@
         <v>0</v>
       </c>
       <c r="N42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O42" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P42" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="Q42" t="n">
         <v>0</v>
       </c>
       <c r="R42" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S42" t="n">
         <v>0</v>
       </c>
       <c r="T42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U42" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V42" t="n">
         <v>2</v>
@@ -3944,12 +3944,12 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Isaiah Brown</t>
+          <t>Hayden Assemian</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>FLA</t>
+          <t>SC</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3966,46 +3966,46 @@
         <v>2</v>
       </c>
       <c r="I43" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J43" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M43" t="n">
         <v>0</v>
       </c>
       <c r="N43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O43" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P43" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="Q43" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R43" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="S43" t="n">
         <v>0</v>
       </c>
       <c r="T43" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U43" t="n">
         <v>1</v>
       </c>
       <c r="V43" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44">
@@ -4026,35 +4026,35 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Jasper Johnson</t>
+          <t>Isaiah Brown</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>UK</t>
+          <t>FLA</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>UGA@UK</t>
+          <t>SC@FLA</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Halftime</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H44" t="n">
         <v>2</v>
       </c>
       <c r="I44" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L44" t="n">
         <v>1</v>
@@ -4066,28 +4066,28 @@
         <v>0</v>
       </c>
       <c r="O44" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P44" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="Q44" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R44" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="S44" t="n">
         <v>0</v>
       </c>
       <c r="T44" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
@@ -4108,7 +4108,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Jordan Ross</t>
+          <t>Kanon Catchings</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -4123,23 +4123,23 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Halftime</t>
+          <t>10:55 - 2nd Half</t>
         </is>
       </c>
       <c r="H45" t="n">
         <v>2</v>
       </c>
       <c r="I45" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J45" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K45" t="n">
         <v>1</v>
       </c>
       <c r="L45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M45" t="n">
         <v>0</v>
@@ -4148,22 +4148,22 @@
         <v>0</v>
       </c>
       <c r="O45" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P45" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="Q45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R45" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="S45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T45" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U45" t="n">
         <v>0</v>
@@ -4190,35 +4190,35 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Brandon Garrison</t>
+          <t>Nic Codie</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>UK</t>
+          <t>TEX</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>UGA@UK</t>
+          <t>LSU@TEX</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Halftime</t>
+          <t>4:59 - 2nd Half</t>
         </is>
       </c>
       <c r="H46" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I46" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J46" t="n">
         <v>1</v>
       </c>
       <c r="K46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L46" t="n">
         <v>0</v>
@@ -4230,28 +4230,28 @@
         <v>0</v>
       </c>
       <c r="O46" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P46" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="Q46" t="n">
         <v>0</v>
       </c>
       <c r="R46" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S46" t="n">
         <v>0</v>
       </c>
       <c r="T46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U46" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V46" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -4272,22 +4272,22 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Nic Codie</t>
+          <t>Jordan Ross</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>TEX</t>
+          <t>UGA</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>LSU@TEX</t>
+          <t>UGA@UK</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>16:16 - 2nd Half</t>
+          <t>10:55 - 2nd Half</t>
         </is>
       </c>
       <c r="H47" t="n">
@@ -4297,13 +4297,13 @@
         <v>0</v>
       </c>
       <c r="J47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K47" t="n">
         <v>1</v>
       </c>
       <c r="L47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M47" t="n">
         <v>0</v>
@@ -4312,16 +4312,16 @@
         <v>0</v>
       </c>
       <c r="O47" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P47" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="Q47" t="n">
         <v>0</v>
       </c>
       <c r="R47" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S47" t="n">
         <v>0</v>
@@ -4354,35 +4354,35 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Trent Noah</t>
+          <t>Rashad King</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>UK</t>
+          <t>LSU</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>UGA@UK</t>
+          <t>LSU@TEX</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Halftime</t>
+          <t>4:59 - 2nd Half</t>
         </is>
       </c>
       <c r="H48" t="n">
         <v>1</v>
       </c>
       <c r="I48" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J48" t="n">
         <v>1</v>
       </c>
       <c r="K48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L48" t="n">
         <v>0</v>
@@ -4397,13 +4397,13 @@
         <v>0</v>
       </c>
       <c r="P48" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="Q48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R48" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S48" t="n">
         <v>0</v>
@@ -4415,7 +4415,7 @@
         <v>0</v>
       </c>
       <c r="V48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -4436,35 +4436,35 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Alex Kovatchev</t>
+          <t>Trent Noah</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>FLA</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>SC@FLA</t>
+          <t>UGA@UK</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Final</t>
+          <t>10:55 - 2nd Half</t>
         </is>
       </c>
       <c r="H49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I49" t="n">
         <v>0</v>
       </c>
       <c r="J49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L49" t="n">
         <v>0</v>
@@ -4479,7 +4479,7 @@
         <v>0</v>
       </c>
       <c r="P49" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="Q49" t="n">
         <v>0</v>
@@ -4497,7 +4497,7 @@
         <v>0</v>
       </c>
       <c r="V49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50">
@@ -4518,7 +4518,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>CJ Ingram</t>
+          <t>Alex Kovatchev</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -4543,7 +4543,7 @@
         <v>0</v>
       </c>
       <c r="J50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K50" t="n">
         <v>0</v>
@@ -4561,13 +4561,13 @@
         <v>0</v>
       </c>
       <c r="P50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q50" t="n">
         <v>0</v>
       </c>
       <c r="R50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S50" t="n">
         <v>0</v>
@@ -4600,12 +4600,12 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Grant Polk</t>
+          <t>CJ Ingram</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>SC</t>
+          <t>FLA</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4625,7 +4625,7 @@
         <v>0</v>
       </c>
       <c r="J51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K51" t="n">
         <v>0</v>
@@ -4643,13 +4643,13 @@
         <v>0</v>
       </c>
       <c r="P51" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q51" t="n">
         <v>0</v>
       </c>
       <c r="R51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S51" t="n">
         <v>0</v>
@@ -4682,22 +4682,22 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Kareem Stagg</t>
+          <t>Grant Polk</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>UGA</t>
+          <t>SC</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>UGA@UK</t>
+          <t>SC@FLA</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Halftime</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H52" t="n">
@@ -4707,37 +4707,37 @@
         <v>0</v>
       </c>
       <c r="J52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K52" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M52" t="n">
         <v>0</v>
       </c>
       <c r="N52" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O52" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P52" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="Q52" t="n">
         <v>0</v>
       </c>
       <c r="R52" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S52" t="n">
         <v>0</v>
       </c>
       <c r="T52" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U52" t="n">
         <v>0</v>
@@ -4764,29 +4764,29 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Nordin Kapic</t>
+          <t>Jasper Johnson</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>SC</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>SC@FLA</t>
+          <t>UGA@UK</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Final</t>
+          <t>10:55 - 2nd Half</t>
         </is>
       </c>
       <c r="H53" t="n">
         <v>0</v>
       </c>
       <c r="I53" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J53" t="n">
         <v>1</v>
@@ -4801,25 +4801,25 @@
         <v>0</v>
       </c>
       <c r="N53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O53" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P53" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="Q53" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R53" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="S53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T53" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="U53" t="n">
         <v>0</v>
@@ -4846,12 +4846,12 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Olivier Rioux</t>
+          <t>Nordin Kapic</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>FLA</t>
+          <t>SC</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4871,13 +4871,13 @@
         <v>0</v>
       </c>
       <c r="J54" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K54" t="n">
         <v>0</v>
       </c>
       <c r="L54" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M54" t="n">
         <v>0</v>
@@ -4886,22 +4886,22 @@
         <v>0</v>
       </c>
       <c r="O54" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P54" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="Q54" t="n">
         <v>0</v>
       </c>
       <c r="R54" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S54" t="n">
         <v>0</v>
       </c>
       <c r="T54" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U54" t="n">
         <v>0</v>
@@ -4928,22 +4928,22 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>PJ Carter</t>
+          <t>Olivier Rioux</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>LSU</t>
+          <t>FLA</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>LSU@TEX</t>
+          <t>SC@FLA</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>16:16 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H55" t="n">
@@ -5010,32 +5010,32 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Viktor Mikic</t>
+          <t>PJ Carter</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>FLA</t>
+          <t>LSU</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>SC@FLA</t>
+          <t>LSU@TEX</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Final</t>
+          <t>4:59 - 2nd Half</t>
         </is>
       </c>
       <c r="H56" t="n">
         <v>0</v>
       </c>
       <c r="I56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K56" t="n">
         <v>0</v>
@@ -5059,19 +5059,19 @@
         <v>0</v>
       </c>
       <c r="R56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S56" t="n">
         <v>0</v>
       </c>
       <c r="T56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V56" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -5092,12 +5092,12 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>EJ Walker</t>
+          <t>Viktor Mikic</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>SC</t>
+          <t>FLA</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -5111,13 +5111,13 @@
         </is>
       </c>
       <c r="H57" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="I57" t="n">
         <v>1</v>
       </c>
       <c r="J57" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K57" t="n">
         <v>0</v>
@@ -5129,25 +5129,25 @@
         <v>0</v>
       </c>
       <c r="N57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O57" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="P57" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="Q57" t="n">
         <v>0</v>
       </c>
       <c r="R57" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="S57" t="n">
         <v>0</v>
       </c>
       <c r="T57" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="U57" t="n">
         <v>1</v>
@@ -5174,32 +5174,32 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Justin Bailey</t>
+          <t>EJ Walker</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>UGA</t>
+          <t>SC</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>UGA@UK</t>
+          <t>SC@FLA</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>Halftime</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H58" t="n">
         <v>-1</v>
       </c>
       <c r="I58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J58" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K58" t="n">
         <v>0</v>
@@ -5211,31 +5211,31 @@
         <v>0</v>
       </c>
       <c r="N58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O58" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="P58" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="Q58" t="n">
         <v>0</v>
       </c>
       <c r="R58" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="S58" t="n">
         <v>0</v>
       </c>
       <c r="T58" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V58" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59">
@@ -5256,7 +5256,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Kanon Catchings</t>
+          <t>Justin Bailey</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -5271,7 +5271,7 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>Halftime</t>
+          <t>10:55 - 2nd Half</t>
         </is>
       </c>
       <c r="H59" t="n">
@@ -5281,7 +5281,7 @@
         <v>0</v>
       </c>
       <c r="J59" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K59" t="n">
         <v>0</v>
@@ -5296,22 +5296,22 @@
         <v>0</v>
       </c>
       <c r="O59" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P59" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="Q59" t="n">
         <v>0</v>
       </c>
       <c r="R59" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="S59" t="n">
         <v>0</v>
       </c>
       <c r="T59" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U59" t="n">
         <v>0</v>
@@ -5338,32 +5338,32 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Rashad King</t>
+          <t>Alex Lloyd</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>LSU</t>
+          <t>FLA</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>LSU@TEX</t>
+          <t>SC@FLA</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>16:16 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H60" t="n">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="I60" t="n">
         <v>0</v>
       </c>
       <c r="J60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K60" t="n">
         <v>0</v>
@@ -5378,28 +5378,28 @@
         <v>0</v>
       </c>
       <c r="O60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P60" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="Q60" t="n">
         <v>0</v>
       </c>
       <c r="R60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S60" t="n">
         <v>0</v>
       </c>
       <c r="T60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U60" t="n">
         <v>0</v>
       </c>
       <c r="V60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61">
@@ -5420,22 +5420,22 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Alex Lloyd</t>
+          <t>Kareem Stagg</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>FLA</t>
+          <t>UGA</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>SC@FLA</t>
+          <t>UGA@UK</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>Final</t>
+          <t>10:55 - 2nd Half</t>
         </is>
       </c>
       <c r="H61" t="n">
@@ -5445,43 +5445,43 @@
         <v>0</v>
       </c>
       <c r="J61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K61" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M61" t="n">
         <v>0</v>
       </c>
       <c r="N61" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O61" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P61" t="n">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="Q61" t="n">
         <v>0</v>
       </c>
       <c r="R61" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="S61" t="n">
         <v>0</v>
       </c>
       <c r="T61" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U61" t="n">
         <v>0</v>
       </c>
       <c r="V61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62">
@@ -5517,7 +5517,7 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>16:16 - 2nd Half</t>
+          <t>4:59 - 2nd Half</t>
         </is>
       </c>
       <c r="H62" t="n">
@@ -5614,7 +5614,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="C2" t="n">
         <v>3</v>
@@ -5627,7 +5627,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="C3" t="n">
         <v>3</v>
@@ -5640,7 +5640,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C4" t="n">
         <v>1</v>
@@ -5649,11 +5649,11 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>The Backslashers</t>
+          <t>Hilton Heads</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C5" t="n">
         <v>1</v>
@@ -5662,11 +5662,11 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Hilton Heads</t>
+          <t>Bend Rimmers</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C6" t="n">
         <v>1</v>
@@ -5675,7 +5675,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Bend Rimmers</t>
+          <t>The Backslashers</t>
         </is>
       </c>
       <c r="B7" t="n">

</xml_diff>